<commit_message>
--Add 1. expr, &&配置。
</commit_message>
<xml_diff>
--- a/Assets/Tables/skill.xlsx
+++ b/Assets/Tables/skill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test\Doom\Assets\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E797B820-AE3B-4901-8157-C8216C24AB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D328AF-C42A-4AC6-ACF6-F976AB1BBD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1110" yWindow="3150" windowWidth="27090" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>0=cast_nova();</t>
+    <t>0=cast_nova()&amp;&amp;cast_twine();</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -466,7 +466,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>